<commit_message>
Update config.json with new session ID and last run date; update Excel files for calibration and PM records
</commit_message>
<xml_diff>
--- a/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
+++ b/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA542"/>
+  <dimension ref="A1:AA545"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -59539,6 +59539,333 @@
       <c r="Z542" t="inlineStr"/>
       <c r="AA542" t="inlineStr"/>
     </row>
+    <row r="543">
+      <c r="A543" t="inlineStr"/>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>425946</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>PYT3_09960</t>
+        </is>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>BME</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr">
+        <is>
+          <t>SOM KONKAEW</t>
+        </is>
+      </c>
+      <c r="F543" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G543" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="H543" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="I543" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="J543" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="K543" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="L543" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="M543" t="inlineStr">
+        <is>
+          <t>566152</t>
+        </is>
+      </c>
+      <c r="N543" t="inlineStr">
+        <is>
+          <t>ITTIPAT IEMDEE</t>
+        </is>
+      </c>
+      <c r="O543" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="P543" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="Q543" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="R543" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="S543" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T543" t="inlineStr"/>
+      <c r="U543" t="inlineStr"/>
+      <c r="V543" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="W543" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="X543" t="inlineStr"/>
+      <c r="Y543" t="inlineStr"/>
+      <c r="Z543" t="inlineStr"/>
+      <c r="AA543" t="inlineStr"/>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr"/>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>109972</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>PYT3_04692</t>
+        </is>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>BME</t>
+        </is>
+      </c>
+      <c r="E544" t="inlineStr">
+        <is>
+          <t>SOM KONKAEW</t>
+        </is>
+      </c>
+      <c r="F544" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G544" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="H544" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="I544" t="inlineStr">
+        <is>
+          <t>24/06/2025</t>
+        </is>
+      </c>
+      <c r="J544" t="inlineStr">
+        <is>
+          <t>24/06/2025</t>
+        </is>
+      </c>
+      <c r="K544" t="inlineStr">
+        <is>
+          <t>24/06/2025</t>
+        </is>
+      </c>
+      <c r="L544" t="inlineStr">
+        <is>
+          <t>24/06/2025</t>
+        </is>
+      </c>
+      <c r="M544" t="inlineStr">
+        <is>
+          <t>566152</t>
+        </is>
+      </c>
+      <c r="N544" t="inlineStr">
+        <is>
+          <t>ITTIPAT IEMDEE</t>
+        </is>
+      </c>
+      <c r="O544" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="P544" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="Q544" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="R544" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="S544" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T544" t="inlineStr"/>
+      <c r="U544" t="inlineStr"/>
+      <c r="V544" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="W544" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="X544" t="inlineStr"/>
+      <c r="Y544" t="inlineStr"/>
+      <c r="Z544" t="inlineStr"/>
+      <c r="AA544" t="inlineStr"/>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr"/>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>40114</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>PYT3_02521</t>
+        </is>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>BME</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr">
+        <is>
+          <t>SOM KONKAEW</t>
+        </is>
+      </c>
+      <c r="F545" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G545" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="H545" t="inlineStr">
+        <is>
+          <t>30/06/2025</t>
+        </is>
+      </c>
+      <c r="I545" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="J545" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="K545" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="L545" t="inlineStr">
+        <is>
+          <t>01/06/2025</t>
+        </is>
+      </c>
+      <c r="M545" t="inlineStr">
+        <is>
+          <t>566152</t>
+        </is>
+      </c>
+      <c r="N545" t="inlineStr">
+        <is>
+          <t>ITTIPAT IEMDEE</t>
+        </is>
+      </c>
+      <c r="O545" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="P545" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="Q545" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="R545" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+      <c r="S545" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T545" t="inlineStr"/>
+      <c r="U545" t="inlineStr"/>
+      <c r="V545" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="W545" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="X545" t="inlineStr"/>
+      <c r="Y545" t="inlineStr"/>
+      <c r="Z545" t="inlineStr"/>
+      <c r="AA545" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: Enhance log output with color-coded messages for better visibility
</commit_message>
<xml_diff>
--- a/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
+++ b/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,14 +571,10 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>430258</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PYT3T_10103</t>
+          <t>PYT3_01766</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -598,27 +594,27 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>01/09/2025</t>
+          <t>01/12/2025</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>30/09/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>4/12/2025</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1/10/2025</t>
+          <t>31/12/2025</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>5/9/2025</t>
+          <t>4/12/2025</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -684,254 +680,6 @@
         </is>
       </c>
       <c r="Z2" t="inlineStr">
-        <is>
-          <t>OPD SURGERY(ศัลยกรรม)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>430259</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>PYT3T_10104</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>BME</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DARANPHOP YIMYAM</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>01/09/2025</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>30/09/2025</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>5/9/2025</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1/10/2025</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>5/9/2025</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>7/1/2026</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>566152</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>ITTIPAT IEMDEE</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>PM doable</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Perform CAL</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>OPD SURGERY(ศัลยกรรม)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>37993</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>PYT3_01766</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>BME</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>SOM KONKAEW</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>01/12/2025</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>4/12/2025</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>4/12/2025</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>4/12/2025</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>7/1/2026</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>566152</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>ITTIPAT IEMDEE</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>PM doable</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Perform CAL</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>SUCCESS</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
         <is>
           <t>GASTROINTESTINAL LABORATORY(GI)</t>
         </is>

</xml_diff>

<commit_message>
fix: Update session ID and last run date in configuration file; update Excel backup records
</commit_message>
<xml_diff>
--- a/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
+++ b/py_test_ui/EXCEL FILE/recordCal_PM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="173">
   <si>
     <t xml:space="preserve">N0</t>
   </si>
@@ -356,6 +356,189 @@
   </si>
   <si>
     <t xml:space="preserve">PYT3_08715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_04921</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">308862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_08097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">276714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_07577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3D_00653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">147092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_05453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_00113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_05923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">297068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_07804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">418280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_09631</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02479_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">289534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_04921_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">289532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_08097_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02479_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02479_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02479_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_00165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_02479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">191703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_06079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_01899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_05840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_06490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">378952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_09048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">408613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_09516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">408614</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_09517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">371802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_08922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_00182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_00221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3_01849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYT3D_00106</t>
   </si>
 </sst>
 </file>
@@ -445,13 +628,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -646,10 +833,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2:AB37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R73" activeCellId="0" sqref="R73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,6 +922,9 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="0" t="s">
         <v>26</v>
       </c>
@@ -797,6 +987,9 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="0" t="s">
         <v>40</v>
       </c>
@@ -859,6 +1052,9 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="0" t="s">
         <v>43</v>
       </c>
@@ -921,6 +1117,9 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="0" t="s">
         <v>45</v>
       </c>
@@ -983,6 +1182,9 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="0" t="s">
         <v>47</v>
       </c>
@@ -1045,6 +1247,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="0" t="s">
         <v>49</v>
       </c>
@@ -1107,6 +1312,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="0" t="s">
         <v>51</v>
       </c>
@@ -1169,6 +1377,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="0" t="s">
         <v>53</v>
       </c>
@@ -1231,6 +1442,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>9</v>
+      </c>
       <c r="B10" s="0" t="s">
         <v>55</v>
       </c>
@@ -1293,6 +1507,9 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>10</v>
+      </c>
       <c r="B11" s="0" t="s">
         <v>57</v>
       </c>
@@ -1355,6 +1572,9 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>11</v>
+      </c>
       <c r="B12" s="0" t="s">
         <v>59</v>
       </c>
@@ -1417,6 +1637,9 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
       <c r="B13" s="0" t="s">
         <v>61</v>
       </c>
@@ -1479,6 +1702,9 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
       <c r="B14" s="0" t="s">
         <v>63</v>
       </c>
@@ -1541,6 +1767,9 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>14</v>
+      </c>
       <c r="B15" s="0" t="s">
         <v>65</v>
       </c>
@@ -1603,6 +1832,9 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
       <c r="B16" s="0" t="s">
         <v>67</v>
       </c>
@@ -1665,6 +1897,9 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
       <c r="B17" s="0" t="s">
         <v>69</v>
       </c>
@@ -1727,6 +1962,9 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>17</v>
+      </c>
       <c r="B18" s="0" t="s">
         <v>71</v>
       </c>
@@ -1789,6 +2027,9 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>18</v>
+      </c>
       <c r="B19" s="0" t="s">
         <v>73</v>
       </c>
@@ -1851,6 +2092,9 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>19</v>
+      </c>
       <c r="B20" s="0" t="s">
         <v>75</v>
       </c>
@@ -1913,6 +2157,9 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>20</v>
+      </c>
       <c r="B21" s="0" t="s">
         <v>77</v>
       </c>
@@ -1975,6 +2222,9 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>21</v>
+      </c>
       <c r="B22" s="0" t="s">
         <v>79</v>
       </c>
@@ -2037,6 +2287,9 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>22</v>
+      </c>
       <c r="B23" s="0" t="s">
         <v>81</v>
       </c>
@@ -2099,6 +2352,9 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>23</v>
+      </c>
       <c r="B24" s="0" t="s">
         <v>83</v>
       </c>
@@ -2161,6 +2417,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>24</v>
+      </c>
       <c r="B25" s="0" t="s">
         <v>85</v>
       </c>
@@ -2223,6 +2482,9 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>25</v>
+      </c>
       <c r="B26" s="0" t="s">
         <v>88</v>
       </c>
@@ -2285,6 +2547,9 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>26</v>
+      </c>
       <c r="B27" s="0" t="s">
         <v>90</v>
       </c>
@@ -2347,6 +2612,9 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>27</v>
+      </c>
       <c r="B28" s="0" t="s">
         <v>92</v>
       </c>
@@ -2409,6 +2677,9 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>28</v>
+      </c>
       <c r="B29" s="0" t="s">
         <v>94</v>
       </c>
@@ -2471,6 +2742,9 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>29</v>
+      </c>
       <c r="B30" s="0" t="s">
         <v>96</v>
       </c>
@@ -2533,6 +2807,9 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="B31" s="0" t="s">
         <v>98</v>
       </c>
@@ -2595,6 +2872,9 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="n">
+        <v>31</v>
+      </c>
       <c r="B32" s="0" t="s">
         <v>100</v>
       </c>
@@ -2657,6 +2937,9 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="n">
+        <v>32</v>
+      </c>
       <c r="B33" s="0" t="s">
         <v>102</v>
       </c>
@@ -2719,6 +3002,9 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="n">
+        <v>33</v>
+      </c>
       <c r="B34" s="0" t="s">
         <v>104</v>
       </c>
@@ -2781,6 +3067,9 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="n">
+        <v>34</v>
+      </c>
       <c r="B35" s="0" t="s">
         <v>106</v>
       </c>
@@ -2843,6 +3132,9 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="n">
+        <v>35</v>
+      </c>
       <c r="B36" s="0" t="s">
         <v>108</v>
       </c>
@@ -2905,6 +3197,9 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="n">
+        <v>36</v>
+      </c>
       <c r="B37" s="0" t="s">
         <v>110</v>
       </c>
@@ -2963,6 +3258,1956 @@
         <v>39</v>
       </c>
       <c r="W37" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M38" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V38" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W38" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M39" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q39" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R39" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V39" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W39" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M40" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q40" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R40" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V40" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W40" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M41" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R41" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V41" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W41" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O42" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q42" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R42" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V42" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W42" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M43" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R43" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V43" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W43" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M44" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O44" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R44" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S44" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V44" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W44" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M45" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N45" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S45" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V45" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W45" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M46" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N46" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O46" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R46" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S46" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W46" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M47" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O47" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P47" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R47" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S47" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W47" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M48" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N48" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O48" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P48" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q48" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R48" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V48" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W48" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M49" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O49" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R49" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S49" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V49" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W49" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M50" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N50" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O50" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P50" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R50" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V50" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W50" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L51" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M51" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O51" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P51" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q51" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R51" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S51" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V51" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W51" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M52" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N52" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O52" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R52" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S52" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W52" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N53" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O53" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R53" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S53" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V53" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W53" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O54" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q54" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R54" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S54" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V54" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W54" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N55" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P55" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R55" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S55" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V55" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W55" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N56" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O56" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q56" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R56" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S56" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V56" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W56" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N57" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O57" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P57" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q57" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R57" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S57" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V57" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W57" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M58" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N58" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O58" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P58" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q58" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R58" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S58" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V58" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W58" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L59" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N59" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O59" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P59" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q59" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R59" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S59" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V59" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W59" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M60" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N60" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O60" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P60" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q60" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R60" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S60" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V60" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W60" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L61" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M61" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N61" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O61" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P61" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q61" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R61" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S61" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V61" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W61" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M62" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N62" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O62" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P62" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q62" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R62" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S62" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V62" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W62" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N63" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O63" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P63" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q63" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R63" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S63" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V63" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W63" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N64" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O64" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P64" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q64" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R64" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S64" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V64" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W64" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N65" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O65" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P65" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R65" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S65" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V65" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W65" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N66" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O66" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P66" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R66" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S66" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V66" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W66" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="M67" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="N67" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O67" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P67" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q67" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R67" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S67" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="V67" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W67" s="0" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>